<commit_message>
correction du new document
</commit_message>
<xml_diff>
--- a/documentation/avancement/bug&opti.xlsx
+++ b/documentation/avancement/bug&opti.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Description </t>
   </si>
@@ -39,9 +39,6 @@
     <t>Le temps où la bombe rougit est mis en brut</t>
   </si>
   <si>
-    <t>il faut que le résultat obtenu soit un entier</t>
-  </si>
-  <si>
     <t>utilisation de Math.Round() du temps_exp /10</t>
   </si>
   <si>
@@ -49,6 +46,12 @@
   </si>
   <si>
     <t xml:space="preserve">Math,Round() existe? </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>il faut que le résultat obtenu soit proportionnel au temps de l'explosion et que cela soit un entier</t>
   </si>
 </sst>
 </file>
@@ -105,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -113,9 +116,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,131 +429,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6">
+        <v>41204</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mise en place du bonus
</commit_message>
<xml_diff>
--- a/documentation/avancement/bug&opti.xlsx
+++ b/documentation/avancement/bug&opti.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">Description </t>
   </si>
@@ -66,9 +66,6 @@
     <t xml:space="preserve">Etat </t>
   </si>
   <si>
-    <t>A corriger</t>
-  </si>
-  <si>
     <t>Plus aucun déplacement par case donc</t>
   </si>
   <si>
@@ -82,6 +79,18 @@
   </si>
   <si>
     <t>Lorsqu'on reste appuyé sur un bout de déplacement l'animation est un petit peu saccadé</t>
+  </si>
+  <si>
+    <t>Timer plus précis</t>
+  </si>
+  <si>
+    <t>Le timer n'est pas le nombre de millisecondes écoulées mais le nombre de fois qu'est passé le code dans tel ou tel boucle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction retournant le nbr de millisecondes depuis le dernier passage dans la boucle doit exister </t>
+  </si>
+  <si>
+    <t>A chercher</t>
   </si>
 </sst>
 </file>
@@ -97,7 +106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +116,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,15 +179,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,212 +511,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="C2" s="7">
         <v>41204</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7">
+        <v>41205</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="I3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5">
+      <c r="C4" s="7">
         <v>41205</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5">
-        <v>41205</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
+      <c r="C5" s="7">
+        <v>41206</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="8"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="8"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="8"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="8"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="9"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="9"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="9"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="9"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="9"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="9"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>